<commit_message>
feat: import file sv ui
</commit_message>
<xml_diff>
--- a/public/files/student_topic_template.xlsx
+++ b/public/files/student_topic_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\HTTT\DoAnTN\Project\FE3\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\HTTT\DoAnTN\Project\FE3\public\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B0A702E9-5660-4F9D-8EA1-1B37955FBC20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F43F0B0C-A2F3-45E1-B616-7A2FFB045E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B8962491-F3BD-455F-A1CF-BA3E487930C5}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{B8962491-F3BD-455F-A1CF-BA3E487930C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>STT</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>lop</t>
+  </si>
+  <si>
+    <t>hodem</t>
   </si>
 </sst>
 </file>
@@ -422,22 +425,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{911FCA87-15F1-4ABC-A4FB-DB4A063AD3B9}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" customWidth="1"/>
-    <col min="3" max="3" width="19.77734375" customWidth="1"/>
-    <col min="4" max="4" width="15.77734375" customWidth="1"/>
-    <col min="5" max="5" width="19.77734375" customWidth="1"/>
+    <col min="2" max="3" width="15.109375" customWidth="1"/>
+    <col min="4" max="4" width="19.77734375" customWidth="1"/>
+    <col min="5" max="5" width="15.77734375" customWidth="1"/>
+    <col min="6" max="6" width="19.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -445,12 +448,15 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>